<commit_message>
Everything is ready for assignment2
</commit_message>
<xml_diff>
--- a/doc/TimeLog.xlsx
+++ b/doc/TimeLog.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Лист2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t xml:space="preserve">action</t>
   </si>
@@ -119,6 +120,54 @@
   </si>
   <si>
     <t xml:space="preserve">15 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimeLog for Assignment 2 to on List 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study the book chapters 4-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 hours </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study the book chapters 6-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Use Case Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw State Machine Diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw Class Diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement The Game / Refactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 hours</t>
   </si>
 </sst>
 </file>
@@ -297,18 +346,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="49.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.89"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
@@ -458,6 +507,11 @@
       </c>
       <c r="E9" s="0" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -469,4 +523,112 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="5" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Iteration 3 commit and push
</commit_message>
<xml_diff>
--- a/doc/TimeLog.xlsx
+++ b/doc/TimeLog.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Лист2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Лист3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t xml:space="preserve">action</t>
   </si>
@@ -168,6 +169,24 @@
   </si>
   <si>
     <t xml:space="preserve">6 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study the book chapters 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5 hours </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Test Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUnit5 Auto test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 hours</t>
   </si>
 </sst>
 </file>
@@ -532,8 +551,8 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -631,4 +650,99 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>